<commit_message>
question paper format changes
</commit_message>
<xml_diff>
--- a/frontend/public/static/sampleexcelsheet.xlsx
+++ b/frontend/public/static/sampleexcelsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\question-paper-generator\frontend\public\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QP generator\frontend\public\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A68F71A-8C97-499F-BCC7-9C26FB4685BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7474C3F2-9C08-432B-A345-6DCB51E74722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA31C51E-0910-4D53-8026-AA7A24C29CD0}"/>
   </bookViews>
@@ -20,19 +20,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>marks</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,7 +377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,12 +385,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EA1CC9-8289-4817-AC93-AEA1A2A06BEE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>